<commit_message>
upload HANA with updated model
</commit_message>
<xml_diff>
--- a/Model/Skus_test.xlsx
+++ b/Model/Skus_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01168fd146a71175/Documents/GitHub/Supply-Chain-Network-Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_C5F27CD0CF2928CEAA160BCE9B9DE6A5502D1504" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E0350C14-9E60-4FCC-871E-DFA338671678}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_C5F27CD0CF2928CEAA160BCE9B9DE6A5502D1504" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34F23D4D-6111-44B2-BA7A-5D32FF3F552B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2003,6 +2003,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>